<commit_message>
updated dummy data with actual data
</commit_message>
<xml_diff>
--- a/properties/entity/User.xlsx
+++ b/properties/entity/User.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>AttributeName</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>InputType</t>
+  </si>
+  <si>
+    <t>ValidationConstraint</t>
+  </si>
+  <si>
+    <t>MaxLength</t>
   </si>
 </sst>
 </file>
@@ -411,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -422,9 +431,12 @@
     <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.90625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,8 +449,17 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -452,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -463,7 +484,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -474,7 +495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -485,7 +506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -499,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -513,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -524,7 +545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>

</xml_diff>